<commit_message>
Report com screenshots implementado.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_bdd/testData/MassaDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-appium-bdd\src\main\java\br\com\rsinet\hub_bdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A110DA-03B4-481F-A326-DEB3679482FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8F49D9-B73F-4D19-B5FF-45483DC0B68F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
@@ -213,7 +213,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>lucascarvalh43</t>
+    <t>lucascarvalh63</t>
   </si>
 </sst>
 </file>

</xml_diff>